<commit_message>
BNS Amendment and Renewal test cases completed
</commit_message>
<xml_diff>
--- a/src/data/TestData.xlsx
+++ b/src/data/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcharles\source\Repository\CDBatch_Migration\CD_PW_Feb\RCBatch\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RC-BatchFile-Automation Folder\RCAutomation-16Jan2026\RC-Smoke\RCBatch\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7A344B-3B46-4EF7-A453-5055ECC58EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C458043E-278E-48C4-A0CC-0415EA29ED7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="InputFileInfo" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">InputFileInfo!$A$1:$T$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">InputFileInfo!$A$1:$V$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>ScenarioId</t>
   </si>
@@ -153,6 +153,24 @@
   </si>
   <si>
     <t>BNS_COMM_DischargeHappyPath</t>
+  </si>
+  <si>
+    <t>BNS_COMM_RenewalHappyPath</t>
+  </si>
+  <si>
+    <t>BNS_Comm_Renewal.xml</t>
+  </si>
+  <si>
+    <t>BNS_COMM_AmendmentHappyPath</t>
+  </si>
+  <si>
+    <t>AmendmentSampleFile</t>
+  </si>
+  <si>
+    <t>BNS_Comm_Amendment.xml</t>
+  </si>
+  <si>
+    <t>AmendmentFileDescription</t>
   </si>
 </sst>
 </file>
@@ -519,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,14 +555,15 @@
     <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="27.109375" customWidth="1"/>
+    <col min="14" max="14" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.88671875" customWidth="1"/>
+    <col min="17" max="17" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,34 +598,40 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -627,11 +652,11 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -651,7 +676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -670,11 +695,11 @@
       <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -693,19 +718,77 @@
       <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>32</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>36</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" t="s">
+        <v>32</v>
+      </c>
+      <c r="R6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" t="s">
+        <v>42</v>
+      </c>
+      <c r="P7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R7" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A1:A2 A6:A1048576">
+  <autoFilter ref="A1:V2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A1:A2 A8:A1048576">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
@@ -714,7 +797,7 @@
   <conditionalFormatting sqref="A4">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
+  <conditionalFormatting sqref="A5:A7">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>